<commit_message>
Multiple Changes inside file Day-2,3 md as Day-5 changed
</commit_message>
<xml_diff>
--- a/Week-6/Day-2/DAY-2-Feature-Engineering-Summary.xlsx
+++ b/Week-6/Day-2/DAY-2-Feature-Engineering-Summary.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Encoding Used</t>
   </si>
   <si>
-    <t xml:space="preserve">OneHotEncoder</t>
+    <t xml:space="preserve">TargetEncoder</t>
   </si>
   <si>
     <t xml:space="preserve">Selection Method</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Correlation &gt; 0.9 removed</t>
   </si>
   <si>
-    <t xml:space="preserve">Top-10 Mutual Information</t>
+    <t xml:space="preserve">Top-25 Mutual Information</t>
   </si>
   <si>
     <t xml:space="preserve">Notes &amp; Insights</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">• Correlation filtering reduced multicollinearity (threshold = 0.9).</t>
   </si>
   <si>
-    <t xml:space="preserve">• Mutual Information Top-10 selection used for stable dimensionality reduction.</t>
+    <t xml:space="preserve">• Mutual Information Top-25 selection used for stable dimensionality reduction.</t>
   </si>
   <si>
     <t xml:space="preserve">• Final dataset is modeling-ready and reproducible.</t>
@@ -101,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +138,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,32 +194,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -412,173 +426,173 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="30"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>225</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>208</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>